<commit_message>
PeaksLoading task; New Functionalities; UI Improvements
Added restart simulation button. Changed isPaused boolean property to top level static field. Added fade transitions to splash screen elements. Completed column to damage hashmap that holds damage state of columns. Various fixes to UI to make it more readable and intuitive. Migrated initializePeaks() top level method to a Task nested within injectStage. Implemented loadingPeaks task/loading-animation when injecting large mixture of peaks. Fixed broken image of chemical data: Cas: 10604-60-1 name: p1-iodoethylbenzene
</commit_message>
<xml_diff>
--- a/docs/worklog.xlsx
+++ b/docs/worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karim\Documents\Education &amp; Self Study\Programming Class\24JavaFX\ChromatographySimulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A343C5-2537-4BB2-A3C2-BAB7AA882C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F9518A-256A-466E-9118-3EDB147D750E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="677" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3057,16 +3057,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>573232</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>516081</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>96485</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>105795</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3089,28 +3089,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15203632" y="133349"/>
-          <a:ext cx="14647718" cy="10059636"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>103910</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>52994</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>356554</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>122189</xdr:rowOff>
+          <a:off x="12098481" y="0"/>
+          <a:ext cx="19848369" cy="13631295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>408710</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>167294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>51754</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>45989</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3133,7 +3133,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1323110" y="243494"/>
+          <a:off x="2847110" y="2072294"/>
           <a:ext cx="13663844" cy="7117695"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4240,8 +4240,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>